<commit_message>
feat: update 2022 plan table and graph xmind
</commit_message>
<xml_diff>
--- a/___/table/Two thousand and twenty-two/Self-taught higher education examinations.xlsx
+++ b/___/table/Two thousand and twenty-two/Self-taught higher education examinations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540" tabRatio="675" firstSheet="3" activeTab="7"/>
+    <workbookView windowWidth="28125" windowHeight="12540" tabRatio="675"/>
   </bookViews>
   <sheets>
     <sheet name="考试流程" sheetId="9" r:id="rId1"/>
@@ -951,9 +951,9 @@
     <numFmt numFmtId="178" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="179" formatCode="0&quot;年&quot;"/>
     <numFmt numFmtId="180" formatCode="0&quot;月&quot;"/>
-    <numFmt numFmtId="181" formatCode="aaa"/>
-    <numFmt numFmtId="182" formatCode="0&quot;日&quot;"/>
-    <numFmt numFmtId="183" formatCode="d"/>
+    <numFmt numFmtId="181" formatCode="0&quot;日&quot;"/>
+    <numFmt numFmtId="182" formatCode="d"/>
+    <numFmt numFmtId="183" formatCode="aaa"/>
   </numFmts>
   <fonts count="71">
     <font>
@@ -1250,7 +1250,7 @@
     <font>
       <u/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Microsoft YaHei"/>
       <charset val="0"/>
     </font>
@@ -3149,7 +3149,7 @@
     <xf numFmtId="180" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3230,19 +3230,19 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="12" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="12" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="12" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="12" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="14" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="14" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="12" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="12" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="12" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="12" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4887,8 +4887,8 @@
   <sheetPr/>
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -7077,7 +7077,7 @@
   <sheetPr/>
   <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -8551,8 +8551,8 @@
   <sheetPr/>
   <dimension ref="B1:AH35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="24" customHeight="1"/>
@@ -10445,7 +10445,7 @@
   <dimension ref="B2:Q32"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.775" defaultRowHeight="22.05" customHeight="1"/>
@@ -10702,14 +10702,14 @@
       </c>
       <c r="D12" s="9">
         <f t="shared" ref="D12:H12" si="4">IFERROR(COUNTIFS(C15:C31,"☑")/COUNTA(D15:D31),"-")</f>
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>163</v>
       </c>
       <c r="F12" s="9">
         <f t="shared" si="4"/>
-        <v>0.0625</v>
+        <v>0.3125</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>163</v>
@@ -10913,7 +10913,7 @@
         <v>182</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>183</v>
@@ -10959,7 +10959,7 @@
         <v>189</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>190</v>
@@ -10999,7 +10999,7 @@
     <row r="19" s="1" customFormat="1" customHeight="1" spans="2:17">
       <c r="B19" s="2"/>
       <c r="C19" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>196</v>
@@ -11179,7 +11179,7 @@
         <v>219</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>220</v>
@@ -11271,7 +11271,7 @@
         <v>233</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>234</v>
@@ -11357,7 +11357,7 @@
     <row r="27" s="1" customFormat="1" customHeight="1" spans="2:17">
       <c r="B27" s="2"/>
       <c r="C27" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>247</v>
@@ -11597,7 +11597,7 @@
     <mergeCell ref="O8:O10"/>
   </mergeCells>
   <conditionalFormatting sqref="N15">
-    <cfRule type="expression" dxfId="11" priority="20">
+    <cfRule type="expression" dxfId="11" priority="17">
       <formula>$E15="☑"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11617,22 +11617,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="expression" dxfId="11" priority="28">
+    <cfRule type="expression" dxfId="11" priority="25">
       <formula>$G31="☑"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31">
-    <cfRule type="expression" dxfId="11" priority="27">
+    <cfRule type="expression" dxfId="11" priority="24">
       <formula>$I31="☑"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L31">
-    <cfRule type="expression" dxfId="11" priority="26">
+    <cfRule type="expression" dxfId="11" priority="23">
       <formula>$K31="☑"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D13">
-    <cfRule type="dataBar" priority="37">
+    <cfRule type="dataBar" priority="64">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11640,7 +11640,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{b5873103-e54e-42c7-b8b3-8cbbbe09b09d}</x14:id>
+          <x14:id>{ecc8d183-2a1a-4068-a522-4ce20ed5e157}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11651,7 +11651,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F13">
-    <cfRule type="dataBar" priority="36">
+    <cfRule type="dataBar" priority="63">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11659,7 +11659,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{49f60bfa-48b4-438d-856e-1e430a49eebe}</x14:id>
+          <x14:id>{cb6b5c3c-e147-4bb5-8fb5-ff52745a6aa4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11670,7 +11670,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H13">
-    <cfRule type="dataBar" priority="35">
+    <cfRule type="dataBar" priority="62">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11678,13 +11678,13 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{d56ddcd2-d80d-490b-b11d-3d995d8826de}</x14:id>
+          <x14:id>{0fd0a591-6fcc-4e06-897d-020678e40687}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:H22">
-    <cfRule type="expression" dxfId="11" priority="23">
+    <cfRule type="expression" dxfId="11" priority="20">
       <formula>$E15="☑"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11694,7 +11694,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J13">
-    <cfRule type="dataBar" priority="34">
+    <cfRule type="dataBar" priority="61">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11702,13 +11702,13 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{40c7f888-68de-40c8-b190-83484c0f0100}</x14:id>
+          <x14:id>{8a5e2590-a789-4a6a-8407-789648e24a45}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:J22">
-    <cfRule type="expression" dxfId="11" priority="22">
+    <cfRule type="expression" dxfId="11" priority="19">
       <formula>$E15="☑"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11718,7 +11718,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12:L13">
-    <cfRule type="dataBar" priority="33">
+    <cfRule type="dataBar" priority="60">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11726,13 +11726,13 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{f99ab3f0-6ffe-4f6e-a19a-bf008c465a22}</x14:id>
+          <x14:id>{a52da99f-a867-4591-b795-0b119adc783d}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15:L22">
-    <cfRule type="expression" dxfId="11" priority="21">
+    <cfRule type="expression" dxfId="11" priority="18">
       <formula>$E15="☑"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11742,7 +11742,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12:N13">
-    <cfRule type="dataBar" priority="32">
+    <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11750,7 +11750,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{e967ca09-331e-473e-8a23-ed7dedbafbb0}</x14:id>
+          <x14:id>{d79a2b32-3a86-4e59-ae43-5e849b27768a}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11781,7 +11781,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P12:P13">
-    <cfRule type="dataBar" priority="31">
+    <cfRule type="dataBar" priority="58">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11789,7 +11789,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{21146c13-b2cf-4b6a-bb05-c6a6d9f4446b}</x14:id>
+          <x14:id>{36855296-8b5c-40ed-af1b-84a531d5718b}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11810,37 +11810,37 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D6 E6:F6 G6:H6 I6:J6 K6:L6 M6:N6 O6:P6">
-    <cfRule type="expression" dxfId="12" priority="38">
+    <cfRule type="expression" dxfId="12" priority="65">
       <formula>C6&lt;=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C10 E8:E10 G8:G10 I8:I10 K8:K10 M8:M10 O8:O10">
-    <cfRule type="expression" dxfId="13" priority="40">
+    <cfRule type="expression" dxfId="13" priority="67">
       <formula>C8&lt;=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9 F9 H9 J9 L9 N9 P9">
-    <cfRule type="expression" dxfId="14" priority="39">
+    <cfRule type="expression" dxfId="14" priority="66">
       <formula>C8&lt;=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:D22 D31">
-    <cfRule type="expression" dxfId="11" priority="30">
+    <cfRule type="expression" dxfId="11" priority="27">
       <formula>$C15="☑"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:F22 F31">
-    <cfRule type="expression" dxfId="11" priority="29">
+    <cfRule type="expression" dxfId="11" priority="26">
       <formula>$E15="☑"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P19:P22 P31">
-    <cfRule type="expression" dxfId="11" priority="24">
+    <cfRule type="expression" dxfId="11" priority="21">
       <formula>$O19="☑"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N21:N22 N31">
-    <cfRule type="expression" dxfId="11" priority="25">
+    <cfRule type="expression" dxfId="11" priority="22">
       <formula>$M21="☑"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11856,7 +11856,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{b5873103-e54e-42c7-b8b3-8cbbbe09b09d}">
+          <x14:cfRule type="dataBar" id="{ecc8d183-2a1a-4068-a522-4ce20ed5e157}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -11871,7 +11871,7 @@
           <xm:sqref>D12:D13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{49f60bfa-48b4-438d-856e-1e430a49eebe}">
+          <x14:cfRule type="dataBar" id="{cb6b5c3c-e147-4bb5-8fb5-ff52745a6aa4}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -11886,7 +11886,7 @@
           <xm:sqref>F12:F13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{d56ddcd2-d80d-490b-b11d-3d995d8826de}">
+          <x14:cfRule type="dataBar" id="{0fd0a591-6fcc-4e06-897d-020678e40687}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -11901,7 +11901,7 @@
           <xm:sqref>H12:H13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{40c7f888-68de-40c8-b190-83484c0f0100}">
+          <x14:cfRule type="dataBar" id="{8a5e2590-a789-4a6a-8407-789648e24a45}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -11916,7 +11916,7 @@
           <xm:sqref>J12:J13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{f99ab3f0-6ffe-4f6e-a19a-bf008c465a22}">
+          <x14:cfRule type="dataBar" id="{a52da99f-a867-4591-b795-0b119adc783d}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -11931,7 +11931,7 @@
           <xm:sqref>L12:L13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{e967ca09-331e-473e-8a23-ed7dedbafbb0}">
+          <x14:cfRule type="dataBar" id="{d79a2b32-3a86-4e59-ae43-5e849b27768a}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -11946,7 +11946,7 @@
           <xm:sqref>N12:N13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{21146c13-b2cf-4b6a-bb05-c6a6d9f4446b}">
+          <x14:cfRule type="dataBar" id="{36855296-8b5c-40ed-af1b-84a531d5718b}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
feat: update today plan table.
</commit_message>
<xml_diff>
--- a/___/table/Two thousand and twenty-two/Self-taught higher education examinations.xlsx
+++ b/___/table/Two thousand and twenty-two/Self-taught higher education examinations.xlsx
@@ -973,14 +973,14 @@
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0&quot;年&quot;"/>
-    <numFmt numFmtId="177" formatCode="mmm\ dd"/>
-    <numFmt numFmtId="178" formatCode="ddd"/>
-    <numFmt numFmtId="179" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="180" formatCode="0&quot;月&quot;"/>
-    <numFmt numFmtId="181" formatCode="0&quot;日&quot;"/>
-    <numFmt numFmtId="182" formatCode="aaa"/>
-    <numFmt numFmtId="183" formatCode="d"/>
+    <numFmt numFmtId="176" formatCode="0&quot;月&quot;"/>
+    <numFmt numFmtId="177" formatCode="d"/>
+    <numFmt numFmtId="178" formatCode="mmm\ dd"/>
+    <numFmt numFmtId="179" formatCode="ddd"/>
+    <numFmt numFmtId="180" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="181" formatCode="0&quot;年&quot;"/>
+    <numFmt numFmtId="182" formatCode="0&quot;日&quot;"/>
+    <numFmt numFmtId="183" formatCode="aaa"/>
   </numFmts>
   <fonts count="72">
     <font>
@@ -3130,13 +3130,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3159,7 +3159,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3171,7 +3171,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3195,13 +3195,13 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="181" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3282,19 +3282,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="13" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="13" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="13" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="13" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="15" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="15" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="13" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="13" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="13" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="13" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5653,8 +5653,8 @@
   <sheetPr/>
   <dimension ref="B1:BO31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.775" defaultRowHeight="14.25"/>
@@ -6622,7 +6622,7 @@
       </c>
       <c r="F12" s="11">
         <f>IFERROR(COUNTIFS(E15:E30,"☑")/COUNTA(F15:F30),"-")</f>
-        <v>0.75</v>
+        <v>0.875</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>163</v>
@@ -7759,7 +7759,7 @@
         <v>248</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>249</v>
@@ -8772,7 +8772,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{82ebb097-024d-4897-ba60-034e79b841fc}</x14:id>
+          <x14:id>{27179fb7-7656-432d-a74d-848f4d256c0b}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8786,7 +8786,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8de637d9-935f-48bb-8179-870c580b8fe4}</x14:id>
+          <x14:id>{02eb2e28-89fe-4f5c-bef0-6536b19aa98d}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8800,7 +8800,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{e42db0e7-176a-4174-92c0-89c0485a7563}</x14:id>
+          <x14:id>{d4b6190c-73f5-482a-a30e-d2ffb101d0ed}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8814,7 +8814,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{b8616de1-6fc9-44b1-98ed-25831e42804e}</x14:id>
+          <x14:id>{ab063935-6dc0-4206-8666-ccf98e9f2643}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8828,7 +8828,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8860ed8b-b691-4c30-a5da-dba97ae49179}</x14:id>
+          <x14:id>{323f74f8-86b4-43fa-b822-93c066efcf04}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8842,7 +8842,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5bebfd58-90b3-41ba-8dc2-58d628daab7f}</x14:id>
+          <x14:id>{2966afed-42e2-4acf-9dc6-a438ceb100d9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8866,7 +8866,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{f9e0f782-d311-4c8a-8f47-68e77832114f}</x14:id>
+          <x14:id>{4884fbce-29c8-4923-88a6-cb5156d31d79}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8883,7 +8883,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{82ebb097-024d-4897-ba60-034e79b841fc}">
+          <x14:cfRule type="dataBar" id="{27179fb7-7656-432d-a74d-848f4d256c0b}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -8898,7 +8898,7 @@
           <xm:sqref>D12:D13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8de637d9-935f-48bb-8179-870c580b8fe4}">
+          <x14:cfRule type="dataBar" id="{02eb2e28-89fe-4f5c-bef0-6536b19aa98d}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -8913,7 +8913,7 @@
           <xm:sqref>F12:F13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{e42db0e7-176a-4174-92c0-89c0485a7563}">
+          <x14:cfRule type="dataBar" id="{d4b6190c-73f5-482a-a30e-d2ffb101d0ed}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -8928,7 +8928,7 @@
           <xm:sqref>H12:H13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{b8616de1-6fc9-44b1-98ed-25831e42804e}">
+          <x14:cfRule type="dataBar" id="{ab063935-6dc0-4206-8666-ccf98e9f2643}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -8943,7 +8943,7 @@
           <xm:sqref>J12:J13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8860ed8b-b691-4c30-a5da-dba97ae49179}">
+          <x14:cfRule type="dataBar" id="{323f74f8-86b4-43fa-b822-93c066efcf04}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -8958,7 +8958,7 @@
           <xm:sqref>L12:L13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5bebfd58-90b3-41ba-8dc2-58d628daab7f}">
+          <x14:cfRule type="dataBar" id="{2966afed-42e2-4acf-9dc6-a438ceb100d9}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -8973,7 +8973,7 @@
           <xm:sqref>N12:N13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{f9e0f782-d311-4c8a-8f47-68e77832114f}">
+          <x14:cfRule type="dataBar" id="{4884fbce-29c8-4923-88a6-cb5156d31d79}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15260,7 +15260,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{eaa351c1-b272-46b1-a89f-fe9db0664a31}</x14:id>
+          <x14:id>{60c2302f-bbf2-406f-a23a-703c58a4a1ef}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15279,7 +15279,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4caee3f7-663d-49f3-813d-36f37680e6b6}</x14:id>
+          <x14:id>{db08d8d4-ed5e-440d-8a10-870bbd1b7a95}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15298,7 +15298,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{f4f1be65-48fa-459c-80c4-08bb32ea9ecc}</x14:id>
+          <x14:id>{0119b0f2-f9fe-41bb-9b88-31e278866c0c}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15322,7 +15322,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{97e87440-613a-4898-9d35-10613886558a}</x14:id>
+          <x14:id>{cfe52207-6fbf-46ca-98d7-4a8bd9d9515a}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15346,7 +15346,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4d1e6ee0-a722-4579-bf63-94522b23e96c}</x14:id>
+          <x14:id>{c8ce488b-b414-4d6b-9434-750ba6d5fab3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15370,7 +15370,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{ce6d959f-f95a-4e6e-b58e-80afbac3e141}</x14:id>
+          <x14:id>{dd3e91cc-b071-4c28-9162-4d697f128635}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15409,7 +15409,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{9ab17b5a-a2d6-4288-9409-26412f6eb4ce}</x14:id>
+          <x14:id>{1e6fdecc-109c-4b9e-9d8e-a41c9793c682}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15476,7 +15476,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{eaa351c1-b272-46b1-a89f-fe9db0664a31}">
+          <x14:cfRule type="dataBar" id="{60c2302f-bbf2-406f-a23a-703c58a4a1ef}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15491,7 +15491,7 @@
           <xm:sqref>D12:D13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4caee3f7-663d-49f3-813d-36f37680e6b6}">
+          <x14:cfRule type="dataBar" id="{db08d8d4-ed5e-440d-8a10-870bbd1b7a95}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15506,7 +15506,7 @@
           <xm:sqref>F12:F13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{f4f1be65-48fa-459c-80c4-08bb32ea9ecc}">
+          <x14:cfRule type="dataBar" id="{0119b0f2-f9fe-41bb-9b88-31e278866c0c}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15521,7 +15521,7 @@
           <xm:sqref>H12:H13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{97e87440-613a-4898-9d35-10613886558a}">
+          <x14:cfRule type="dataBar" id="{cfe52207-6fbf-46ca-98d7-4a8bd9d9515a}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15536,7 +15536,7 @@
           <xm:sqref>J12:J13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4d1e6ee0-a722-4579-bf63-94522b23e96c}">
+          <x14:cfRule type="dataBar" id="{c8ce488b-b414-4d6b-9434-750ba6d5fab3}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15551,7 +15551,7 @@
           <xm:sqref>L12:L13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{ce6d959f-f95a-4e6e-b58e-80afbac3e141}">
+          <x14:cfRule type="dataBar" id="{dd3e91cc-b071-4c28-9162-4d697f128635}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15566,7 +15566,7 @@
           <xm:sqref>N12:N13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{9ab17b5a-a2d6-4288-9409-26412f6eb4ce}">
+          <x14:cfRule type="dataBar" id="{1e6fdecc-109c-4b9e-9d8e-a41c9793c682}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
feat: add higher education examinations long study plan.
</commit_message>
<xml_diff>
--- a/___/table/Two thousand and twenty-two/Self-taught higher education examinations.xlsx
+++ b/___/table/Two thousand and twenty-two/Self-taught higher education examinations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="13400" tabRatio="675" firstSheet="5" activeTab="9"/>
+    <workbookView windowWidth="30240" windowHeight="13300" tabRatio="675" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="考试流程" sheetId="9" r:id="rId1"/>
@@ -969,18 +969,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="12">
-    <numFmt numFmtId="176" formatCode="aaa"/>
-    <numFmt numFmtId="177" formatCode="d"/>
-    <numFmt numFmtId="178" formatCode="0&quot;日&quot;"/>
-    <numFmt numFmtId="179" formatCode="0&quot;月&quot;"/>
+    <numFmt numFmtId="176" formatCode="0&quot;日&quot;"/>
+    <numFmt numFmtId="177" formatCode="aaa"/>
+    <numFmt numFmtId="178" formatCode="0&quot;月&quot;"/>
+    <numFmt numFmtId="179" formatCode="0&quot;年&quot;"/>
     <numFmt numFmtId="180" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="181" formatCode="ddd"/>
+    <numFmt numFmtId="182" formatCode="mmm\ dd"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="183" formatCode="d"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="ddd"/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="182" formatCode="0&quot;年&quot;"/>
-    <numFmt numFmtId="183" formatCode="mmm\ dd"/>
   </numFmts>
   <fonts count="72">
     <font>
@@ -1321,14 +1321,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1343,14 +1336,50 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1365,30 +1394,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -1398,14 +1403,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1419,17 +1417,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1441,16 +1441,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1547,73 +1547,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1631,7 +1583,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1643,7 +1607,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1655,7 +1685,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1667,25 +1703,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1697,37 +1721,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2871,8 +2871,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2881,7 +2881,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2916,21 +2931,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -2938,15 +2938,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2965,6 +2956,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2972,94 +2972,94 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="52" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="25" borderId="98" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="58" fillId="17" borderId="96" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="23" borderId="98" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="66" fillId="24" borderId="96" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="68" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="56" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="99" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="62" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="41" borderId="101" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="64" fillId="27" borderId="100" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="23" borderId="97" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="24" borderId="98" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="95" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="101" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3068,29 +3068,29 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="52" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="53" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="96" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="97" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3099,22 +3099,22 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="95" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="101" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="94" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="95" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="100" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="94" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3124,10 +3124,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="183" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="181" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3174,7 +3174,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3249,15 +3249,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3276,10 +3276,10 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="13" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="13" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="13" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="13" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3291,13 +3291,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="183" fontId="15" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="13" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="13" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="13" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="13" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3475,7 +3475,7 @@
     <xf numFmtId="0" fontId="22" fillId="11" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3484,7 +3484,7 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3493,23 +3493,23 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="51" xfId="38" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3542,16 +3542,16 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="54" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="54" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="55" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="55" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="56" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="57" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="39" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3593,16 +3593,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="39" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3617,22 +3617,22 @@
     <xf numFmtId="49" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="70" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="70" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="40" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="72" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="72" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="70" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="40" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="73" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="73" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="74" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3647,7 +3647,7 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="75" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="75" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3659,13 +3659,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="63" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="63" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="52" xfId="38" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3675,103 +3675,103 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="76" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="76" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="4" borderId="77" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="78" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="78" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="79" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="79" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="79" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="4" borderId="79" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="80" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="81" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="79" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="79" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="80" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="83" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="78" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="81" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="79" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="78" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="79" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="79" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="83" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="79" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="79" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="80" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="82" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="79" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="84" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="85" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="85" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="78" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="79" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="79" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="79" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="79" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="79" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="80" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="79" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="84" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="85" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="85" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="62" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="79" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="79" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="83" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3780,7 +3780,7 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="86" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="87" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="87" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="74" xfId="38" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3790,59 +3790,59 @@
     <xf numFmtId="0" fontId="45" fillId="4" borderId="88" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="64" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="64" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="89" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="89" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="64" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="64" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="89" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="4" borderId="89" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="90" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="91" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="90" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="89" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="92" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="89" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="89" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="90" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="64" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="89" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="91" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="93" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="90" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="92" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="89" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="64" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="89" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="93" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="1"/>
-    <cellStyle name="常规 4" xfId="2"/>
+    <cellStyle name="常规 4" xfId="1"/>
+    <cellStyle name="常规 2" xfId="2"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="3" builtinId="52"/>
     <cellStyle name="20% - 强调文字颜色 4" xfId="4" builtinId="42"/>
     <cellStyle name="强调文字颜色 4" xfId="5" builtinId="41"/>
@@ -5656,7 +5656,7 @@
   <sheetPr/>
   <dimension ref="B1:BO31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -8776,7 +8776,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{0eb50ea3-1813-44d9-bb3d-b586c104e1fe}</x14:id>
+          <x14:id>{c7becb24-7de3-4a48-8d6b-d4b8126b5af9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8790,7 +8790,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{556154cf-7032-4309-b8de-b3ec2294650c}</x14:id>
+          <x14:id>{b398cd28-54cb-4707-ba09-0bf7e473c110}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8804,7 +8804,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{94c824c0-ac36-43f1-8864-30b139b61da3}</x14:id>
+          <x14:id>{228828ae-f054-465e-afac-183e5b70926c}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8818,7 +8818,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{295ed428-c632-427e-8f31-55eb40a40fd7}</x14:id>
+          <x14:id>{92ec4185-1949-44df-8ddc-6ba6ef9be1a0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8832,7 +8832,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{be2bfb49-139a-461e-9afd-64a1657a984a}</x14:id>
+          <x14:id>{1cb7a964-c8bf-49cc-9a82-61981cd14aa4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8846,7 +8846,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1f79158a-a353-4a8a-b1f1-96591b507447}</x14:id>
+          <x14:id>{750e4cfc-1808-4033-b706-edb1aad22656}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8870,7 +8870,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{08f6c89e-fd96-4279-a05c-6610e2ef5f09}</x14:id>
+          <x14:id>{bc72bc14-e27d-42d0-96a0-bc5552935750}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8887,7 +8887,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{0eb50ea3-1813-44d9-bb3d-b586c104e1fe}">
+          <x14:cfRule type="dataBar" id="{c7becb24-7de3-4a48-8d6b-d4b8126b5af9}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -8902,7 +8902,7 @@
           <xm:sqref>D12:D13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{556154cf-7032-4309-b8de-b3ec2294650c}">
+          <x14:cfRule type="dataBar" id="{b398cd28-54cb-4707-ba09-0bf7e473c110}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -8917,7 +8917,7 @@
           <xm:sqref>F12:F13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{94c824c0-ac36-43f1-8864-30b139b61da3}">
+          <x14:cfRule type="dataBar" id="{228828ae-f054-465e-afac-183e5b70926c}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -8932,7 +8932,7 @@
           <xm:sqref>H12:H13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{295ed428-c632-427e-8f31-55eb40a40fd7}">
+          <x14:cfRule type="dataBar" id="{92ec4185-1949-44df-8ddc-6ba6ef9be1a0}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -8947,7 +8947,7 @@
           <xm:sqref>J12:J13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{be2bfb49-139a-461e-9afd-64a1657a984a}">
+          <x14:cfRule type="dataBar" id="{1cb7a964-c8bf-49cc-9a82-61981cd14aa4}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -8962,7 +8962,7 @@
           <xm:sqref>L12:L13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1f79158a-a353-4a8a-b1f1-96591b507447}">
+          <x14:cfRule type="dataBar" id="{750e4cfc-1808-4033-b706-edb1aad22656}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -8977,7 +8977,7 @@
           <xm:sqref>N12:N13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{08f6c89e-fd96-4279-a05c-6610e2ef5f09}">
+          <x14:cfRule type="dataBar" id="{bc72bc14-e27d-42d0-96a0-bc5552935750}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -10083,8 +10083,8 @@
   <sheetPr/>
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -15264,7 +15264,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{d769a5c5-84cc-4d0a-8c21-236c0f22214c}</x14:id>
+          <x14:id>{69f31f50-813a-48e8-9465-b97973271c3d}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15283,7 +15283,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{0491d15d-3e8e-422b-964f-7bfa7c7657bb}</x14:id>
+          <x14:id>{d198db2f-1884-45ed-92fd-f98830e71eea}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15302,7 +15302,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{fdad7444-eb85-4054-b835-5ef8c630c65d}</x14:id>
+          <x14:id>{01dd88ba-a9f7-4ecf-b1a2-a31debb32680}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15326,7 +15326,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{b7439065-40f9-4a96-8fd9-500777567429}</x14:id>
+          <x14:id>{e0d5bb54-1bab-4dfa-91d1-6b3f1d870771}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15350,7 +15350,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{eee4ebfd-3ced-4c53-b3f5-1e662658b4b6}</x14:id>
+          <x14:id>{6d33ff89-c5a3-48c9-98b6-f5b5f3340797}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15374,7 +15374,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3a201e56-c31d-40ca-8cde-468469b09853}</x14:id>
+          <x14:id>{69a32ced-093a-4bae-b168-7b9b307baee2}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15413,7 +15413,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{492ab1e4-5c7f-43fe-8a38-7497e3caf421}</x14:id>
+          <x14:id>{5b0c66e2-c9e7-491c-8cdd-d2c5e22d751a}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -15480,7 +15480,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{d769a5c5-84cc-4d0a-8c21-236c0f22214c}">
+          <x14:cfRule type="dataBar" id="{69f31f50-813a-48e8-9465-b97973271c3d}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15495,7 +15495,7 @@
           <xm:sqref>D12:D13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{0491d15d-3e8e-422b-964f-7bfa7c7657bb}">
+          <x14:cfRule type="dataBar" id="{d198db2f-1884-45ed-92fd-f98830e71eea}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15510,7 +15510,7 @@
           <xm:sqref>F12:F13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{fdad7444-eb85-4054-b835-5ef8c630c65d}">
+          <x14:cfRule type="dataBar" id="{01dd88ba-a9f7-4ecf-b1a2-a31debb32680}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15525,7 +15525,7 @@
           <xm:sqref>H12:H13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{b7439065-40f9-4a96-8fd9-500777567429}">
+          <x14:cfRule type="dataBar" id="{e0d5bb54-1bab-4dfa-91d1-6b3f1d870771}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15540,7 +15540,7 @@
           <xm:sqref>J12:J13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{eee4ebfd-3ced-4c53-b3f5-1e662658b4b6}">
+          <x14:cfRule type="dataBar" id="{6d33ff89-c5a3-48c9-98b6-f5b5f3340797}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15555,7 +15555,7 @@
           <xm:sqref>L12:L13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3a201e56-c31d-40ca-8cde-468469b09853}">
+          <x14:cfRule type="dataBar" id="{69a32ced-093a-4bae-b168-7b9b307baee2}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -15570,7 +15570,7 @@
           <xm:sqref>N12:N13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{492ab1e4-5c7f-43fe-8a38-7497e3caf421}">
+          <x14:cfRule type="dataBar" id="{5b0c66e2-c9e7-491c-8cdd-d2c5e22d751a}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>